<commit_message>
Update example model specification sheets
</commit_message>
<xml_diff>
--- a/model_specifications/test_parameters_base.xlsx
+++ b/model_specifications/test_parameters_base.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brchan\Documents\Github\Lymphoma Model\model_specifications\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Brandon\Documents\GitHub\monte_carlo_markov\model_specifications\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB32B33-5176-4406-8C7B-5E19B35544C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="11265" yWindow="1545" windowWidth="17295" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="transitions" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="32">
   <si>
     <t>start_state</t>
   </si>
@@ -117,12 +118,15 @@
   </si>
   <si>
     <t>remission_asct</t>
+  </si>
+  <si>
+    <t>static</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -456,10 +460,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -594,61 +598,73 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="1" max="2" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2">
         <v>350</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
-        <v>0</v>
+      <c r="B3" t="s">
+        <v>31</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
-        <v>0</v>
+      <c r="B4" t="s">
+        <v>31</v>
       </c>
       <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
         <v>0</v>
       </c>
     </row>
@@ -658,60 +674,72 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="1" max="2" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2">
         <v>0.85</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3">
         <v>1</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
-        <v>0</v>
+      <c r="B4" t="s">
+        <v>31</v>
       </c>
       <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
         <v>0</v>
       </c>
     </row>
@@ -721,7 +749,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -780,7 +808,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -863,7 +891,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Update example input spreadsheets
</commit_message>
<xml_diff>
--- a/model_specifications/test_parameters_base.xlsx
+++ b/model_specifications/test_parameters_base.xlsx
@@ -1,31 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Brandon\Documents\GitHub\monte_carlo_markov\model_specifications\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB32B33-5176-4406-8C7B-5E19B35544C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B8CE31-4E4F-4153-AD35-DC4766D1C9A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11265" yWindow="1545" windowWidth="17295" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5085" yWindow="1740" windowWidth="21075" windowHeight="12585" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="transitions" sheetId="1" r:id="rId1"/>
     <sheet name="costs" sheetId="2" r:id="rId2"/>
     <sheet name="utilities" sheetId="3" r:id="rId3"/>
     <sheet name="specification" sheetId="4" r:id="rId4"/>
-    <sheet name="condensed_states" sheetId="5" r:id="rId5"/>
-    <sheet name="state_mappings" sheetId="6" r:id="rId6"/>
+    <sheet name="state_mappings" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="21">
   <si>
     <t>start_state</t>
   </si>
@@ -85,39 +84,6 @@
   </si>
   <si>
     <t>name_start_state</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>mapping</t>
-  </si>
-  <si>
-    <t>treatment_bv_low</t>
-  </si>
-  <si>
-    <t>treatment_bv</t>
-  </si>
-  <si>
-    <t>treatment_bv_med</t>
-  </si>
-  <si>
-    <t>treatment_bv_high</t>
-  </si>
-  <si>
-    <t>rest_bv</t>
-  </si>
-  <si>
-    <t>rest</t>
-  </si>
-  <si>
-    <t>rest_</t>
-  </si>
-  <si>
-    <t>remission_bv</t>
-  </si>
-  <si>
-    <t>remission_asct</t>
   </si>
   <si>
     <t>static</t>
@@ -601,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,7 +597,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>350</v>
@@ -645,7 +611,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -659,7 +625,7 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -706,7 +672,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>0.85</v>
@@ -720,7 +686,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -734,7 +700,7 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -808,93 +774,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
Structural update + more
- Modified code to be more flexible in running models and more modular
- Added support for a method of probabilistic time-dependent transition probabilites
- Revamped example notebooks
- Revamped example sepcification excel sheets
- Added example scripts for those who don't use Jupyter/want to use Jupyter
- Cleaned up code
</commit_message>
<xml_diff>
--- a/model_specifications/test_parameters_base.xlsx
+++ b/model_specifications/test_parameters_base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Brandon\Documents\GitHub\monte_carlo_markov\model_specifications\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B8CE31-4E4F-4153-AD35-DC4766D1C9A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0EE382-2ED2-453C-8606-CAF21C4D6391}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5085" yWindow="1740" windowWidth="21075" windowHeight="12585" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11550" yWindow="2610" windowWidth="12540" windowHeight="12585" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="transitions" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="24">
   <si>
     <t>start_state</t>
   </si>
@@ -87,6 +87,15 @@
   </si>
   <si>
     <t>static</t>
+  </si>
+  <si>
+    <t>parameter_3</t>
+  </si>
+  <si>
+    <t>parameter_4</t>
+  </si>
+  <si>
+    <t>notes</t>
   </si>
 </sst>
 </file>
@@ -427,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,11 +447,14 @@
     <col min="1" max="1" width="11.85546875" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
     <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -458,8 +470,17 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -476,7 +497,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -493,7 +514,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -510,7 +531,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -527,7 +548,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -544,7 +565,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -565,10 +586,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,7 +599,7 @@
     <col min="6" max="6" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -591,8 +612,11 @@
       <c r="D1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -606,7 +630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -620,7 +644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -641,10 +665,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,7 +677,7 @@
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -666,8 +690,11 @@
       <c r="D1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -681,7 +708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -695,7 +722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -777,7 +804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated CEA examples. Added NMB and improved model arm summary outputs
NMB calculation added to cost-effectiveness analysis notebook. Model arm summaries now print CIs using simple method
</commit_message>
<xml_diff>
--- a/model_specifications/test_parameters_base.xlsx
+++ b/model_specifications/test_parameters_base.xlsx
@@ -1,30 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Brandon\Documents\GitHub\monte_carlo_markov\model_specifications\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0EE382-2ED2-453C-8606-CAF21C4D6391}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{082D5B47-E41B-4E23-BAC2-AD16B681663C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11550" yWindow="2610" windowWidth="12540" windowHeight="12585" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="1200" windowWidth="11700" windowHeight="13875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="transitions" sheetId="1" r:id="rId1"/>
     <sheet name="costs" sheetId="2" r:id="rId2"/>
     <sheet name="utilities" sheetId="3" r:id="rId3"/>
     <sheet name="specification" sheetId="4" r:id="rId4"/>
-    <sheet name="state_mappings" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="24">
   <si>
     <t>start_state</t>
   </si>
@@ -44,58 +43,58 @@
     <t>treatment</t>
   </si>
   <si>
+    <t>remission</t>
+  </si>
+  <si>
+    <t>death</t>
+  </si>
+  <si>
+    <t>constant</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>cost_variance</t>
+  </si>
+  <si>
+    <t>utility</t>
+  </si>
+  <si>
+    <t>utility_variance</t>
+  </si>
+  <si>
+    <t>max_iterations</t>
+  </si>
+  <si>
+    <t>time_horizon</t>
+  </si>
+  <si>
+    <t>cycle_length</t>
+  </si>
+  <si>
+    <t>discount_rate</t>
+  </si>
+  <si>
+    <t>name_start_state</t>
+  </si>
+  <si>
+    <t>static</t>
+  </si>
+  <si>
+    <t>parameter_3</t>
+  </si>
+  <si>
+    <t>parameter_4</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
     <t>beta</t>
-  </si>
-  <si>
-    <t>remission</t>
-  </si>
-  <si>
-    <t>death</t>
-  </si>
-  <si>
-    <t>constant</t>
-  </si>
-  <si>
-    <t>state</t>
-  </si>
-  <si>
-    <t>cost</t>
-  </si>
-  <si>
-    <t>cost_variance</t>
-  </si>
-  <si>
-    <t>utility</t>
-  </si>
-  <si>
-    <t>utility_variance</t>
-  </si>
-  <si>
-    <t>max_iterations</t>
-  </si>
-  <si>
-    <t>time_horizon</t>
-  </si>
-  <si>
-    <t>cycle_length</t>
-  </si>
-  <si>
-    <t>discount_rate</t>
-  </si>
-  <si>
-    <t>name_start_state</t>
-  </si>
-  <si>
-    <t>static</t>
-  </si>
-  <si>
-    <t>parameter_3</t>
-  </si>
-  <si>
-    <t>parameter_4</t>
-  </si>
-  <si>
-    <t>notes</t>
   </si>
 </sst>
 </file>
@@ -113,15 +112,24 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -134,16 +142,16 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -151,10 +159,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -439,14 +449,14 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" customWidth="1"/>
@@ -455,129 +465,148 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="D2" s="1">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1">
+        <v>100</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1">
+        <v>70</v>
+      </c>
+      <c r="E3" s="1">
+        <v>100</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1">
+        <v>20</v>
+      </c>
+      <c r="E4" s="1">
+        <v>100</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2">
-        <v>10</v>
-      </c>
-      <c r="E2">
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1">
+        <v>50</v>
+      </c>
+      <c r="E5" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>70</v>
-      </c>
-      <c r="E3">
+      <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="1">
+        <v>50</v>
+      </c>
+      <c r="E6" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4">
-        <v>20</v>
-      </c>
-      <c r="E4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5">
-        <v>50</v>
-      </c>
-      <c r="E5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6">
-        <v>50</v>
-      </c>
-      <c r="E6">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>1</v>
       </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -589,7 +618,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,63 +629,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>23</v>
+      <c r="E1" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1">
         <v>350</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -668,7 +700,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,63 +710,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>23</v>
+      <c r="E1" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1">
         <v>0.85</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -746,7 +781,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,7 +792,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1">
         <v>1000</v>
@@ -765,7 +800,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -773,7 +808,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>60</v>
@@ -781,7 +816,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <v>1.4999999999999999E-2</v>
@@ -789,57 +824,13 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B1" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Refreshed examples and added CE quadrant counter
- Refreshed example Jupyter notebooks
- Added convenience function to count points in each quadrant of the CE plane
- Fixed small bug in check_excel() involving eligible types of transitions
</commit_message>
<xml_diff>
--- a/model_specifications/test_parameters_base.xlsx
+++ b/model_specifications/test_parameters_base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Brandon\Documents\GitHub\monte_carlo_markov\model_specifications\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{082D5B47-E41B-4E23-BAC2-AD16B681663C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BDE5BE4-B4F4-4D7F-BB54-41354DA68634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1200" windowWidth="11700" windowHeight="13875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="975" yWindow="3000" windowWidth="25185" windowHeight="11940" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="transitions" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="27">
   <si>
     <t>start_state</t>
   </si>
@@ -95,6 +95,15 @@
   </si>
   <si>
     <t>beta</t>
+  </si>
+  <si>
+    <t>parameter_5</t>
+  </si>
+  <si>
+    <t>parameter_6</t>
+  </si>
+  <si>
+    <t>parameter_7</t>
   </si>
 </sst>
 </file>
@@ -446,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,11 +469,11 @@
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" customWidth="1"/>
+    <col min="7" max="10" width="12.42578125" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -487,10 +496,19 @@
         <v>21</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -509,8 +527,11 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -529,8 +550,11 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -549,8 +573,11 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -569,8 +596,11 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -589,8 +619,11 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -607,6 +640,9 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -618,7 +654,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,7 +817,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>